<commit_message>
update querryTianyan tot 7
</commit_message>
<xml_diff>
--- a/data-raw/public-site/observe-station/xlsx/list-most-year-2019.xlsx
+++ b/data-raw/public-site/observe-station/xlsx/list-most-year-2019.xlsx
@@ -65,7 +65,7 @@
     <t xml:space="preserve">广西环江农田生态系统国家野外科学观测研究站</t>
   </si>
   <si>
-    <t xml:space="preserve">中科院亚热带农业生态研究所</t>
+    <t xml:space="preserve">中国科学院亚热带农业生态研究所</t>
   </si>
   <si>
     <t xml:space="preserve">中科院</t>
@@ -77,7 +77,7 @@
     <t xml:space="preserve">黑龙江三江沼泽湿地生态系统国家野外科学观测研究站</t>
   </si>
   <si>
-    <t xml:space="preserve">中科院东北地理与农业生态研究所</t>
+    <t xml:space="preserve">中国科学院东北地理与农业生态研究所</t>
   </si>
   <si>
     <t xml:space="preserve">5</t>
@@ -86,7 +86,7 @@
     <t xml:space="preserve">湖北神农架森林生态系统国家野外科学观测研究站</t>
   </si>
   <si>
-    <t xml:space="preserve">中科院植物研究所</t>
+    <t xml:space="preserve">中国科学院植物研究所</t>
   </si>
   <si>
     <t xml:space="preserve">6</t>
@@ -101,7 +101,7 @@
     <t xml:space="preserve">山东胶州湾海洋生态系统国家野外科学观测研究站</t>
   </si>
   <si>
-    <t xml:space="preserve">中科院海洋研究所</t>
+    <t xml:space="preserve">中国科学院海洋研究所</t>
   </si>
   <si>
     <t xml:space="preserve">8</t>
@@ -110,7 +110,7 @@
     <t xml:space="preserve">山东禹城农田生态系统国家野外科学观测研究站</t>
   </si>
   <si>
-    <t xml:space="preserve">中科院地理科学与资源研究所</t>
+    <t xml:space="preserve">中国科学院地理科学与资源研究所</t>
   </si>
   <si>
     <t xml:space="preserve">9</t>
@@ -119,7 +119,7 @@
     <t xml:space="preserve">河南封丘农田生态系统国家野外科学观测研究站</t>
   </si>
   <si>
-    <t xml:space="preserve">中科院南京土壤研究所</t>
+    <t xml:space="preserve">中国科学院南京土壤研究所</t>
   </si>
   <si>
     <t xml:space="preserve">10</t>
@@ -134,7 +134,7 @@
     <t xml:space="preserve">吉林长白山森林生态系统国家野外科学观测研究站</t>
   </si>
   <si>
-    <t xml:space="preserve">中科院沈阳应用生态研究所</t>
+    <t xml:space="preserve">中国科学院沈阳应用生态研究所</t>
   </si>
   <si>
     <t xml:space="preserve">12</t>
@@ -143,7 +143,7 @@
     <t xml:space="preserve">四川贡嘎山森林生态系统国家野外科学观测研究站</t>
   </si>
   <si>
-    <t xml:space="preserve">中科院水利部成都山地灾害与环境研究所</t>
+    <t xml:space="preserve">中国科学院水利部成都山地灾害与环境研究所</t>
   </si>
   <si>
     <t xml:space="preserve">13</t>
@@ -152,7 +152,7 @@
     <t xml:space="preserve">广东鼎湖山森林生态系统国家野外科学观测研究站</t>
   </si>
   <si>
-    <t xml:space="preserve">中科院华南植物园</t>
+    <t xml:space="preserve">中国科学院华南植物园</t>
   </si>
   <si>
     <t xml:space="preserve">14</t>
@@ -161,7 +161,7 @@
     <t xml:space="preserve">宁夏沙坡头沙漠生态系统国家野外科学观测研究站</t>
   </si>
   <si>
-    <t xml:space="preserve">中科院寒区旱区环境与工程研究所</t>
+    <t xml:space="preserve">中国科学院寒区旱区环境与工程研究所</t>
   </si>
   <si>
     <t xml:space="preserve">15</t>
@@ -170,7 +170,7 @@
     <t xml:space="preserve">江苏太湖湖泊生态系统国家野外科学观测研究站</t>
   </si>
   <si>
-    <t xml:space="preserve">中科院南京地理与湖泊研究所</t>
+    <t xml:space="preserve">中国科学院南京地理与湖泊研究所</t>
   </si>
   <si>
     <t xml:space="preserve">16</t>
@@ -218,7 +218,7 @@
     <t xml:space="preserve">中国科学技术大学、安徽省地震局</t>
   </si>
   <si>
-    <t xml:space="preserve">中科院 地震局</t>
+    <t xml:space="preserve">中科院、地震局</t>
   </si>
   <si>
     <t xml:space="preserve">21</t>
@@ -227,7 +227,7 @@
     <t xml:space="preserve">北京空间环境国家野外科学观测研究站</t>
   </si>
   <si>
-    <t xml:space="preserve">中科院地质与地球物理研究所</t>
+    <t xml:space="preserve">中国科学院地质与地球物理研究所</t>
   </si>
   <si>
     <t xml:space="preserve">22</t>
@@ -236,7 +236,7 @@
     <t xml:space="preserve">海南空间天气国家野外科学观测研究站</t>
   </si>
   <si>
-    <t xml:space="preserve">中科院空间科学与应用研究中心</t>
+    <t xml:space="preserve">中国科学院空间科学与应用研究中心</t>
   </si>
   <si>
     <t xml:space="preserve">23</t>
@@ -299,7 +299,7 @@
     <t xml:space="preserve">广东大亚湾海洋生态系统国家野外科学观测研究站</t>
   </si>
   <si>
-    <t xml:space="preserve">中科院南海海洋研究所</t>
+    <t xml:space="preserve">中国科学院南海海洋研究所</t>
   </si>
   <si>
     <t xml:space="preserve">30</t>
@@ -314,7 +314,7 @@
     <t xml:space="preserve">河北栾城农田生态系统国家野外科学观测研究站</t>
   </si>
   <si>
-    <t xml:space="preserve">中科院遗传与发育生物学研究所</t>
+    <t xml:space="preserve">中国科学院遗传与发育生物学研究所</t>
   </si>
   <si>
     <t xml:space="preserve">32</t>
@@ -359,10 +359,10 @@
     <t xml:space="preserve">陕西长武农田生态系统国家野外科学观测研究站</t>
   </si>
   <si>
-    <t xml:space="preserve">中科院水利部水土保持研究所</t>
-  </si>
-  <si>
-    <t xml:space="preserve">中科院 教育部</t>
+    <t xml:space="preserve">中国科学院水利部水土保持研究所</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中科院、教育部</t>
   </si>
   <si>
     <t xml:space="preserve">39</t>
@@ -371,7 +371,7 @@
     <t xml:space="preserve">四川盐亭农田生态系统国家野外科学观测研究站</t>
   </si>
   <si>
-    <t xml:space="preserve">中科院 水利部</t>
+    <t xml:space="preserve">中科院、水利部</t>
   </si>
   <si>
     <t xml:space="preserve">40</t>
@@ -386,7 +386,7 @@
     <t xml:space="preserve">新疆策勒荒漠草地生态系统国家野外科学观测研究站</t>
   </si>
   <si>
-    <t xml:space="preserve">中科院新疆生态与地理研究所</t>
+    <t xml:space="preserve">中国科学院新疆生态与地理研究所</t>
   </si>
   <si>
     <t xml:space="preserve">42</t>
@@ -395,7 +395,7 @@
     <t xml:space="preserve">云南哀牢山森林生态系统国家野外科学观测研究站</t>
   </si>
   <si>
-    <t xml:space="preserve">中科院西双版纳热带植物园</t>
+    <t xml:space="preserve">中国科学院西双版纳热带植物园</t>
   </si>
   <si>
     <t xml:space="preserve">43</t>
@@ -419,7 +419,7 @@
     <t xml:space="preserve">东北林业大学</t>
   </si>
   <si>
-    <t xml:space="preserve">教育部 林草局</t>
+    <t xml:space="preserve">教育部、林草局</t>
   </si>
   <si>
     <t xml:space="preserve">46</t>
@@ -443,7 +443,7 @@
     <t xml:space="preserve">中南林业科技大学</t>
   </si>
   <si>
-    <t xml:space="preserve">湖南省科技厅 林草局</t>
+    <t xml:space="preserve">湖南省科技厅、林草局</t>
   </si>
   <si>
     <t xml:space="preserve">48</t>
@@ -467,7 +467,7 @@
     <t xml:space="preserve">青海海北高寒草地生态系统国家野外科学观测研究站</t>
   </si>
   <si>
-    <t xml:space="preserve">中科院西北高原生物研究所</t>
+    <t xml:space="preserve">中国科学院西北高原生物研究所</t>
   </si>
   <si>
     <t xml:space="preserve">51</t>
@@ -482,7 +482,7 @@
     <t xml:space="preserve">湖北东湖湖泊生态系统国家野外科学观测研究站</t>
   </si>
   <si>
-    <t xml:space="preserve">中科院水生生物研究所</t>
+    <t xml:space="preserve">中国科学院水生生物研究所</t>
   </si>
   <si>
     <t xml:space="preserve">53</t>
@@ -584,10 +584,10 @@
     <t xml:space="preserve">湖北武汉引力与固体潮国家野外科学观测研究站</t>
   </si>
   <si>
-    <t xml:space="preserve">中国地震局地震研究所华中科技大学</t>
-  </si>
-  <si>
-    <t xml:space="preserve">地震局 教育部</t>
+    <t xml:space="preserve">中国地震局地震研究所、华中科技大学</t>
+  </si>
+  <si>
+    <t xml:space="preserve">地震局、教育部</t>
   </si>
   <si>
     <t xml:space="preserve">64</t>
@@ -596,7 +596,7 @@
     <t xml:space="preserve">甘肃兰州地球物理国家野外科学观测研究站</t>
   </si>
   <si>
-    <t xml:space="preserve">中国地震局兰州地震研究所甘肃省地震局</t>
+    <t xml:space="preserve">中国地震局兰州地震研究所、甘肃省地震局</t>
   </si>
   <si>
     <t xml:space="preserve">65</t>
@@ -605,7 +605,7 @@
     <t xml:space="preserve">山西太原大陆裂谷动力学国家野外科学观测研究站</t>
   </si>
   <si>
-    <t xml:space="preserve">中国地震局地质研究所山西省地震局</t>
+    <t xml:space="preserve">中国地震局地质研究所、山西省地震局</t>
   </si>
   <si>
     <t xml:space="preserve">66</t>
@@ -614,7 +614,7 @@
     <t xml:space="preserve">湖北武汉大地测量国家野外科学观测研究站</t>
   </si>
   <si>
-    <t xml:space="preserve">中科院测量与地球物理研究所</t>
+    <t xml:space="preserve">中国科学院测量与地球物理研究所</t>
   </si>
   <si>
     <t xml:space="preserve">67</t>
@@ -809,7 +809,7 @@
     <t xml:space="preserve">西藏羊八井宇宙线国家野外科学观测研究站</t>
   </si>
   <si>
-    <t xml:space="preserve">中科院高能物理研究所</t>
+    <t xml:space="preserve">中国科学院高能物理研究所</t>
   </si>
   <si>
     <t xml:space="preserve">91</t>
@@ -818,7 +818,7 @@
     <t xml:space="preserve">西藏拉萨地球物理国家野外科学观测研究站</t>
   </si>
   <si>
-    <t xml:space="preserve">中国地震局地质研究所西藏自治区地震局</t>
+    <t xml:space="preserve">中国地震局地质研究所、西藏自治区地震局</t>
   </si>
   <si>
     <t xml:space="preserve">92</t>
@@ -848,7 +848,7 @@
     <t xml:space="preserve">辽宁沈阳土壤大气环境材料腐蚀国家野外科学观测研究站</t>
   </si>
   <si>
-    <t xml:space="preserve">中科院金属研究所</t>
+    <t xml:space="preserve">中国科学院金属研究所</t>
   </si>
   <si>
     <t xml:space="preserve">95</t>

</xml_diff>